<commit_message>
get_station_info() test passed, get_switch_info() test passed
</commit_message>
<xml_diff>
--- a/test procedure.xlsx
+++ b/test procedure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7fb2c76d2a3db151/Documents/ECE1140/ece1140/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{3F628AAF-80A5-4BFA-B251-539A2752620C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA813AD4-5152-45DF-AA32-13C8240F4891}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{3F628AAF-80A5-4BFA-B251-539A2752620C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D47017D2-F64E-495F-A458-DF7B4D54F4D0}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10980" xr2:uid="{664EECA8-6B58-4079-AB8C-C8AEC57D27CF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>Test Case</t>
   </si>
@@ -220,6 +220,19 @@
   </si>
   <si>
     <t>Red Line has a total of 76 blocks</t>
+  </si>
+  <si>
+    <t>New tables in SQL database are created</t>
+  </si>
+  <si>
+    <t>New track model has 3 lines</t>
+  </si>
+  <si>
+    <t>1) Select track model file
+2) Click import</t>
+  </si>
+  <si>
+    <t>3 tables (Blue Line, Red Line, and Green Line) are created in the SQL database</t>
   </si>
 </sst>
 </file>
@@ -263,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -277,6 +290,9 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -597,15 +613,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3EDDBEF-2379-40C5-810D-8F6D60B79781}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="26.2265625" customWidth="1"/>
+    <col min="1" max="1" width="39.6796875" customWidth="1"/>
     <col min="2" max="2" width="29.1328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="26.31640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.2265625" bestFit="1" customWidth="1"/>
@@ -633,7 +649,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -641,19 +657,23 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:6" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A3" s="6" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="4"/>
+        <v>51</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="7">
+        <v>44893</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" s="4"/>
@@ -664,196 +684,236 @@
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="59" x14ac:dyDescent="0.75">
-      <c r="A8" s="2" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="59" x14ac:dyDescent="0.75">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A9" s="1" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="73.75" x14ac:dyDescent="0.75">
-      <c r="A10" s="2" t="s">
+    <row r="14" spans="1:6" ht="73.75" x14ac:dyDescent="0.75">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="59" x14ac:dyDescent="0.75">
-      <c r="A11" s="2" t="s">
+    <row r="15" spans="1:6" ht="59" x14ac:dyDescent="0.75">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A12" s="2" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="73.75" x14ac:dyDescent="0.75">
-      <c r="A13" s="2" t="s">
+    <row r="17" spans="1:6" ht="73.75" x14ac:dyDescent="0.75">
+      <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="59" x14ac:dyDescent="0.75">
-      <c r="A14" s="2" t="s">
+    <row r="18" spans="1:6" ht="59" x14ac:dyDescent="0.75">
+      <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A15" s="1" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="103.25" x14ac:dyDescent="0.75">
-      <c r="A16" s="2" t="s">
+    <row r="20" spans="1:6" ht="103.25" x14ac:dyDescent="0.75">
+      <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F20" s="5">
         <v>44892</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="103.25" x14ac:dyDescent="0.75">
-      <c r="A17" s="2" t="s">
+    <row r="21" spans="1:6" ht="103.25" x14ac:dyDescent="0.75">
+      <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F21" s="5">
         <v>44892</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="103.25" x14ac:dyDescent="0.75">
-      <c r="A18" s="2" t="s">
+    <row r="22" spans="1:6" ht="103.25" x14ac:dyDescent="0.75">
+      <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F22" s="5">
         <v>44892</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A20" s="1" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A21" s="2" t="s">
+    <row r="25" spans="1:6" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="59" x14ac:dyDescent="0.75">
-      <c r="A22" s="2" t="s">
+    <row r="26" spans="1:6" ht="59" x14ac:dyDescent="0.75">
+      <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A23" s="1" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>